<commit_message>
Added final brood table .xlsx
</commit_message>
<xml_diff>
--- a/Syrah/outputFiles/Annual Summary/2018 Bristol Bay Run Summary Updated 10.23.18_cc.xlsx
+++ b/Syrah/outputFiles/Annual Summary/2018 Bristol Bay Run Summary Updated 10.23.18_cc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/curryc2/Documents/Curry's SYRAH Work/Bristol-Bay-Run-Recon/Syrah/outputFiles/Annual Summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA268400-ABF4-3D45-B5F9-FD6A367471B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E82A85-7ECF-A845-A05B-2A871D4719E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="24000" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38560" yWindow="0" windowWidth="38400" windowHeight="24000" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Run Summary for 2016" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -1167,7 +1167,7 @@
   <dxfs count="3">
     <dxf>
       <fill>
-        <patternFill patternType="solid">
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -1181,7 +1181,7 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
+        <patternFill patternType="solid">
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -9347,7 +9347,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F38706AA-6AAE-1648-8909-366F220205E6}" name="PivotTable1" cacheId="5" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="6" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F38706AA-6AAE-1648-8909-366F220205E6}" name="PivotTable1" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="6" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1" fieldListSortAscending="1">
   <location ref="A5:R92" firstHeaderRow="1" firstDataRow="2" firstDataCol="4" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="18">
     <pivotField axis="axisPage" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1">
@@ -10322,7 +10322,7 @@
     <dataField name="Sum of NA" fld="13" baseField="0" baseItem="0" numFmtId="3"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="0">
+    <format dxfId="2">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1" selected="0" defaultSubtotal="1">
@@ -10340,7 +10340,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="0">
       <pivotArea dataOnly="0" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0" selected="0"/>
@@ -15454,7 +15454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAB5EFB-AFC7-4E0D-A1E7-A65CFFCD7DBD}">
   <dimension ref="A1:W111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -20670,8 +20670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90D183B0-03C9-9142-8BBC-BF733BA4CEB1}">
   <dimension ref="A1:Y109"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="T107" sqref="T107:T109"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="E108" sqref="E108:R108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -24481,7 +24481,7 @@
         <v>62439316</v>
       </c>
     </row>
-    <row r="99" spans="20:23">
+    <row r="99" spans="5:23">
       <c r="V99" s="53">
         <f>V91+V84+V77+V60+V40</f>
         <v>4486292</v>
@@ -24490,24 +24490,138 @@
         <v>143</v>
       </c>
     </row>
-    <row r="101" spans="20:23">
+    <row r="101" spans="5:23">
       <c r="T101" s="53"/>
       <c r="V101" s="53">
         <f>(V94-V99)-V88</f>
         <v>36581406</v>
       </c>
     </row>
-    <row r="102" spans="20:23">
+    <row r="102" spans="5:23">
       <c r="T102" s="53"/>
     </row>
-    <row r="103" spans="20:23">
+    <row r="103" spans="5:23">
       <c r="T103" s="53"/>
       <c r="V103" s="53">
         <f>V101+T101</f>
         <v>36581406</v>
       </c>
     </row>
-    <row r="107" spans="20:23">
+    <row r="105" spans="5:23">
+      <c r="E105" s="69"/>
+      <c r="F105" s="70">
+        <v>439.15771812080573</v>
+      </c>
+      <c r="G105" s="70">
+        <v>280589.47178663453</v>
+      </c>
+      <c r="H105" s="70"/>
+      <c r="I105" s="70">
+        <v>225297.29490441782</v>
+      </c>
+      <c r="J105" s="70">
+        <v>1624.1435001113282</v>
+      </c>
+      <c r="K105" s="70"/>
+      <c r="L105" s="70"/>
+      <c r="M105" s="70"/>
+      <c r="N105" s="70">
+        <v>3819.9320907153469</v>
+      </c>
+      <c r="O105" s="70"/>
+      <c r="P105" s="70"/>
+      <c r="Q105" s="70"/>
+      <c r="R105" s="71">
+        <v>511769.99999999977</v>
+      </c>
+    </row>
+    <row r="106" spans="5:23">
+      <c r="E106" s="69">
+        <v>407.88502894954507</v>
+      </c>
+      <c r="F106" s="70"/>
+      <c r="G106" s="70">
+        <v>307868.43535610475</v>
+      </c>
+      <c r="H106" s="70"/>
+      <c r="I106" s="70">
+        <v>544395.12707690208</v>
+      </c>
+      <c r="J106" s="70">
+        <v>2990.2517397492893</v>
+      </c>
+      <c r="K106" s="70"/>
+      <c r="L106" s="70">
+        <v>7078.3181516399563</v>
+      </c>
+      <c r="M106" s="70"/>
+      <c r="N106" s="70">
+        <v>5959.9826466543891</v>
+      </c>
+      <c r="O106" s="70"/>
+      <c r="P106" s="70"/>
+      <c r="Q106" s="70"/>
+      <c r="R106" s="71">
+        <v>868700</v>
+      </c>
+    </row>
+    <row r="107" spans="5:23">
+      <c r="E107" t="str">
+        <f>E6</f>
+        <v>03</v>
+      </c>
+      <c r="F107" t="str">
+        <f t="shared" ref="F107:R107" si="0">F6</f>
+        <v>11</v>
+      </c>
+      <c r="G107" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H107" t="str">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="I107" t="str">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="J107" t="str">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="K107" t="str">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="L107" t="str">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="M107" t="str">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="N107" t="str">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="O107" t="str">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="P107" t="str">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="Q107" t="str">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="R107" t="str">
+        <f t="shared" si="0"/>
+        <v>Grand Total</v>
+      </c>
       <c r="T107" s="94" t="s">
         <v>144</v>
       </c>
@@ -24516,7 +24630,63 @@
         <v>1380469.9999999998</v>
       </c>
     </row>
-    <row r="108" spans="20:23">
+    <row r="108" spans="5:23">
+      <c r="E108" s="53">
+        <f>SUM(E105:E106)</f>
+        <v>407.88502894954507</v>
+      </c>
+      <c r="F108" s="53">
+        <f t="shared" ref="F108:R108" si="1">SUM(F105:F106)</f>
+        <v>439.15771812080573</v>
+      </c>
+      <c r="G108" s="53">
+        <f t="shared" si="1"/>
+        <v>588457.90714273928</v>
+      </c>
+      <c r="H108" s="53">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I108" s="53">
+        <f t="shared" si="1"/>
+        <v>769692.4219813199</v>
+      </c>
+      <c r="J108" s="53">
+        <f t="shared" si="1"/>
+        <v>4614.3952398606179</v>
+      </c>
+      <c r="K108" s="53">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L108" s="53">
+        <f t="shared" si="1"/>
+        <v>7078.3181516399563</v>
+      </c>
+      <c r="M108" s="53">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N108" s="53">
+        <f t="shared" si="1"/>
+        <v>9779.914737369736</v>
+      </c>
+      <c r="O108" s="53">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P108" s="53">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q108" s="53">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R108" s="53">
+        <f t="shared" si="1"/>
+        <v>1380469.9999999998</v>
+      </c>
       <c r="T108" s="94" t="s">
         <v>145</v>
       </c>
@@ -24525,7 +24695,7 @@
         <v>36581406</v>
       </c>
     </row>
-    <row r="109" spans="20:23">
+    <row r="109" spans="5:23">
       <c r="T109" s="94" t="s">
         <v>146</v>
       </c>

</xml_diff>